<commit_message>
added forests and SVMs
</commit_message>
<xml_diff>
--- a/spotify_3/Data/scores_of_models.xlsx
+++ b/spotify_3/Data/scores_of_models.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cyrusrustomji/Documents/metis/personal_metis/projects/music_3/spotify/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76D2CA9E-4FEC-7540-A64A-6A1131C92816}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D74737AA-BD66-1442-BCC4-D1272F30A52B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{938C0615-05CD-374C-872C-926DEBA5BABB}"/>
   </bookViews>
@@ -25,12 +25,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Linear Regression</t>
   </si>
   <si>
     <t>Score</t>
+  </si>
+  <si>
+    <t>Logistic Regression</t>
+  </si>
+  <si>
+    <t>Gradient Descent</t>
+  </si>
+  <si>
+    <t>KNN</t>
+  </si>
+  <si>
+    <t>SVM</t>
+  </si>
+  <si>
+    <t>Trees</t>
+  </si>
+  <si>
+    <t>Type of Model</t>
+  </si>
+  <si>
+    <t>82% if in order</t>
   </si>
 </sst>
 </file>
@@ -74,9 +95,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -392,28 +414,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EACA7EAC-FBF4-1745-AAAD-A30431084861}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>0.40600000000000003</v>
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.36</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>